<commit_message>
kosten nog aangevuld met details
</commit_message>
<xml_diff>
--- a/kosten.xlsx
+++ b/kosten.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA67E30A-B45C-4EF6-9B1F-356191608D41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A87C293-66CD-46E2-97BF-49DFD822FE57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Bluetooth module</t>
   </si>
@@ -136,15 +136,6 @@
     <t>10 nF smd condensator</t>
   </si>
   <si>
-    <t>kostprijs exclusief lipo, wielen en frame</t>
-  </si>
-  <si>
-    <t>wielen, frame, lipo, ge3d printe stukken</t>
-  </si>
-  <si>
-    <t>pcb prijs</t>
-  </si>
-  <si>
     <t>Aantal</t>
   </si>
   <si>
@@ -167,6 +158,39 @@
   </si>
   <si>
     <t>aansluit draden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deze kostenberekening is gebaseerd op prijzen die terug te vinden zijn op het internet  </t>
+  </si>
+  <si>
+    <t>Om een duidelijk onderscheid te maken: 2 tabellen gemaakt</t>
+  </si>
+  <si>
+    <t>Lipo batterij</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Wielen (4 stuks)</t>
+  </si>
+  <si>
+    <t>Prijslijst FabLab</t>
+  </si>
+  <si>
+    <t>Banggood</t>
+  </si>
+  <si>
+    <t>prijzen kunnen in werkelijkheid variëren aangezien we enkel de exacte aankoopprijs kennen van onze eigen aangkochte materialen</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Ge3Dprinte stukken (PLA Filament)</t>
+  </si>
+  <si>
+    <t>Dubbelzijdige Koper plaat voor PCB</t>
   </si>
 </sst>
 </file>
@@ -174,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_ [$€-413]\ * #,##0.00_ ;_ [$€-413]\ * \-#,##0.00_ ;_ [$€-413]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$€-413]\ * #,##0.00_ ;_ [$€-413]\ * \-#,##0.00_ ;_ [$€-413]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -302,12 +326,12 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,15 +340,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
@@ -339,11 +354,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -627,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:G46"/>
+  <dimension ref="A3:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,32 +667,32 @@
   <sheetData>
     <row r="3" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>1.55</v>
       </c>
       <c r="F6" s="8">
@@ -682,7 +706,7 @@
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>0.2</v>
       </c>
       <c r="F7" s="8">
@@ -696,7 +720,7 @@
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>0.11</v>
       </c>
       <c r="F8" s="8">
@@ -710,7 +734,7 @@
       <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>1.17</v>
       </c>
       <c r="F9" s="8">
@@ -724,7 +748,7 @@
       <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>1.44</v>
       </c>
       <c r="F10" s="8">
@@ -738,7 +762,7 @@
       <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>1.89</v>
       </c>
       <c r="F11" s="8">
@@ -752,7 +776,7 @@
       <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>7.8E-2</v>
       </c>
       <c r="F12" s="8">
@@ -764,9 +788,9 @@
     </row>
     <row r="13" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="17">
+        <v>41</v>
+      </c>
+      <c r="E13" s="14">
         <f>E6+E7+E8+E9+E10+E11+E12*F12</f>
         <v>6.8280000000000003</v>
       </c>
@@ -775,35 +799,35 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>0.1</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -811,13 +835,13 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>1.21</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <v>2</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -825,13 +849,13 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="13">
         <v>1.1399999999999999</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="11">
         <v>2</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -839,13 +863,13 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="13">
         <v>0.02</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -853,13 +877,13 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="13">
         <v>0.08</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <v>5</v>
       </c>
       <c r="G21" s="7" t="s">
@@ -867,13 +891,13 @@
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="13">
         <v>0.05</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="11">
         <v>6</v>
       </c>
       <c r="G22" s="7" t="s">
@@ -881,13 +905,13 @@
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="13">
         <v>0.02</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="11">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
@@ -895,13 +919,13 @@
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F24" s="14">
+      <c r="E24" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F24" s="11">
         <v>2</v>
       </c>
       <c r="G24" s="7" t="s">
@@ -909,13 +933,13 @@
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F25" s="14">
+      <c r="E25" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F25" s="11">
         <v>2</v>
       </c>
       <c r="G25" s="7" t="s">
@@ -923,13 +947,13 @@
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F26" s="14">
+      <c r="E26" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F26" s="11">
         <v>2</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -937,13 +961,13 @@
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F27" s="14">
+      <c r="E27" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F27" s="11">
         <v>9</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -951,13 +975,13 @@
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F28" s="14">
+      <c r="E28" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F28" s="11">
         <v>4</v>
       </c>
       <c r="G28" s="7" t="s">
@@ -965,13 +989,13 @@
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F29" s="14">
+      <c r="E29" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F29" s="11">
         <v>3</v>
       </c>
       <c r="G29" s="7" t="s">
@@ -979,13 +1003,13 @@
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F30" s="14">
+      <c r="E30" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F30" s="11">
         <v>2</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -993,13 +1017,13 @@
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="11">
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
@@ -1007,13 +1031,13 @@
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F32" s="15">
+      <c r="E32" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F32" s="12">
         <v>6</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -1021,13 +1045,13 @@
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F33" s="15">
+      <c r="E33" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F33" s="12">
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
@@ -1035,13 +1059,13 @@
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F34" s="15">
+      <c r="E34" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F34" s="12">
         <v>2</v>
       </c>
       <c r="G34" s="7" t="s">
@@ -1049,13 +1073,13 @@
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F35" s="15">
+      <c r="E35" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F35" s="12">
         <v>6</v>
       </c>
       <c r="G35" s="7" t="s">
@@ -1063,13 +1087,13 @@
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F36" s="15">
+      <c r="E36" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F36" s="12">
         <v>6</v>
       </c>
       <c r="G36" s="7" t="s">
@@ -1077,13 +1101,13 @@
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F37" s="15">
+      <c r="E37" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F37" s="12">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
@@ -1091,13 +1115,13 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F38" s="15">
+      <c r="E38" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F38" s="12">
         <v>3</v>
       </c>
       <c r="G38" s="7" t="s">
@@ -1105,66 +1129,159 @@
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F39" s="15">
+      <c r="E39" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="F39" s="12">
         <v>6</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="13" t="s">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="13">
+        <v>20</v>
+      </c>
+      <c r="F40" s="12">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="13">
+        <v>1.28</v>
+      </c>
+      <c r="F41" s="12">
+        <v>4</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="13">
+        <v>86.1</v>
+      </c>
+      <c r="F42" s="12">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="13">
+        <v>13</v>
+      </c>
+      <c r="F43" s="12">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="13">
+        <v>23.4</v>
+      </c>
+      <c r="F44" s="12">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="13">
+        <v>3.14</v>
+      </c>
+      <c r="F45" s="12">
+        <v>1</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="13">
         <v>0.68</v>
       </c>
-      <c r="F40" s="15">
-        <v>1</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="17">
-        <f>E17*F17+E18*F18+E19*F19+E20*F20+E21*F21+E22*F22+E23*F23+E24*F24+E25*F25+E26*F26+E27*F27+E28*F28+E29*F29+E30*F30+E31*F31+E32*F32+E33*F33+E34*F34+E35*F35+E36*F36+E37*F37+E38*F38+E39*F39+E40*F40</f>
-        <v>6.8399999999999954</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="12" t="s">
+      <c r="F46" s="12">
+        <v>1</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="14">
+        <f>E17*F17+E18*F18+E19*F19+E20*F20+E21*F21+E22*F22+E23*F23+E24*F24+E25*F25+E26*F26+E27*F27+E28*F28+E29*F29+E30*F30+E31*F31+E32*F32+E33*F33+E34*F34+E35*F35+E36*F36+E37*F37+E38*F38+E39*F39+E46*F46+E40*F40+E42*F42+E43*F43+E44*F44+E45*F45+E41*F41</f>
+        <v>157.6</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="4">
+        <f>E47+E13</f>
+        <v>164.428</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="6"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="4">
-        <f>E41+E13</f>
-        <v>13.667999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>